<commit_message>
Konecne doplneni dat mrtve doby
</commit_message>
<xml_diff>
--- a/Harmonogram_aktivita_MD.xlsx
+++ b/Harmonogram_aktivita_MD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Ptacek_Daniel\Mereni_mrtve_doby_VU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\mrtva_doba_VU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA669627-300D-411B-9D52-C2C03E20669D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA8072-3430-49DD-A81F-90B381014517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{F6E2B69B-A5E7-E14B-A240-E694F51C9F54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F6E2B69B-A5E7-E14B-A240-E694F51C9F54}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Datum</t>
   </si>
@@ -141,6 +152,9 @@
   <si>
     <t>viz obrazky v galerii - 4,2 %</t>
   </si>
+  <si>
+    <t>nastaveno na 131J</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -568,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -627,7 +641,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2348,16 +2361,16 @@
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45481.614583333336</v>
       </c>
@@ -2395,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>45482.614583333336</v>
       </c>
@@ -2419,7 +2432,7 @@
         <v>45481.614583333336</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45483.614583333336</v>
       </c>
@@ -2438,7 +2451,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>45484.614583333336</v>
       </c>
@@ -2459,7 +2472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45485.574999999997</v>
       </c>
@@ -2480,7 +2493,7 @@
         <v>8.02</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45486.614583333336</v>
       </c>
@@ -2498,7 +2511,7 @@
         <v>6.2999999999956344</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45487.914583333331</v>
       </c>
@@ -2516,7 +2529,7 @@
         <v>7.0381944444452529</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>45488.652777777781</v>
       </c>
@@ -2534,7 +2547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45489.614583333336</v>
       </c>
@@ -2546,13 +2559,13 @@
         <f t="shared" si="2"/>
         <v>30.41576102211593</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="12">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45490.614583333336</v>
       </c>
@@ -2569,11 +2582,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45491.614583333336</v>
       </c>
@@ -2585,13 +2598,13 @@
         <f t="shared" si="2"/>
         <v>26.648239391123013</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="12">
         <f t="shared" si="1"/>
         <v>11.142361111109494</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>45492.756944444445</v>
       </c>
@@ -2609,7 +2622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45493.614583333336</v>
       </c>
@@ -2621,13 +2634,13 @@
         <f t="shared" si="2"/>
         <v>19.107139052344621</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="12">
         <f t="shared" si="1"/>
         <v>13.022222222221899</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45494.636805555558</v>
       </c>
@@ -2645,7 +2658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45495.614583333336</v>
       </c>
@@ -2663,7 +2676,7 @@
         <v>15.006944444445253</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45496.621527777781</v>
       </c>
@@ -2675,13 +2688,13 @@
         <f t="shared" si="2"/>
         <v>17.412896732966203</v>
       </c>
-      <c r="D17" s="28"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="12">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45497.614583333336</v>
       </c>
@@ -2699,7 +2712,7 @@
         <v>17.169444444443798</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>45498.78402777778</v>
       </c>
@@ -2717,7 +2730,7 @@
         <v>17.635416666664241</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45499.25</v>
       </c>
@@ -2735,7 +2748,7 @@
         <v>18.635416666664241</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>45500.25</v>
       </c>
@@ -2753,7 +2766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45501.614583333336</v>
       </c>
@@ -2771,7 +2784,7 @@
         <v>20.59375</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>45502.208333333336</v>
       </c>
@@ -2783,13 +2796,13 @@
         <f t="shared" si="2"/>
         <v>6.2219265498958407</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="12">
         <f t="shared" si="1"/>
         <v>22.21875</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>45503.833333333336</v>
       </c>
@@ -2807,7 +2820,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>45504.614583333336</v>
       </c>
@@ -2825,7 +2838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>45505.614583333336</v>
       </c>
@@ -2843,7 +2856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>45506.614583333336</v>
       </c>
@@ -2861,7 +2874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>45507.614583333336</v>
       </c>
@@ -2879,7 +2892,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>45508.614583333336</v>
       </c>
@@ -2897,7 +2910,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>45509.614583333336</v>
       </c>
@@ -2915,7 +2928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>45510.614583333336</v>
       </c>
@@ -2933,7 +2946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>45511.614583333336</v>
       </c>
@@ -2951,7 +2964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>45512.614583333336</v>
       </c>
@@ -2969,7 +2982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>45513.614583333336</v>
       </c>
@@ -2987,7 +3000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>45514.614583333336</v>
       </c>
@@ -3005,7 +3018,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>45515.614583333336</v>
       </c>
@@ -3023,7 +3036,7 @@
         <v>35.061111111106584</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>45516.675694444442</v>
       </c>
@@ -3041,7 +3054,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>45517.614583333336</v>
       </c>
@@ -3059,7 +3072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>45518.614583333336</v>
       </c>
@@ -3077,7 +3090,7 @@
         <v>38.024305555554747</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>45519.638888888891</v>
       </c>
@@ -3095,7 +3108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>45520.614583333336</v>
       </c>
@@ -3113,7 +3126,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>45521.614583333336</v>
       </c>
@@ -3131,7 +3144,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>45522.614583333336</v>
       </c>
@@ -3149,7 +3162,7 @@
         <v>42.059027777773736</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>45523.673611111109</v>
       </c>
@@ -3167,7 +3180,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>45524.614583333336</v>
       </c>
@@ -3185,7 +3198,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45525.614583333336</v>
       </c>
@@ -3203,7 +3216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45526.614583333336</v>
       </c>
@@ -3221,7 +3234,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>45527.614583333336</v>
       </c>
@@ -3239,7 +3252,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>45528.614583333336</v>
       </c>
@@ -3257,7 +3270,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>45529.614583333336</v>
       </c>
@@ -3275,7 +3288,7 @@
         <v>48.987499999995634</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>45530.602083333331</v>
       </c>
@@ -3293,7 +3306,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>45531.614583333336</v>
       </c>
@@ -3311,7 +3324,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>45532.614583333336</v>
       </c>
@@ -3329,7 +3342,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>45533.614583333336</v>
       </c>
@@ -3347,7 +3360,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>45534.614583333336</v>
       </c>
@@ -3365,7 +3378,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>45535.614583333336</v>
       </c>
@@ -3383,7 +3396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>45536.614583333336</v>
       </c>
@@ -3401,7 +3414,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>45537.614583333336</v>
       </c>
@@ -3419,7 +3432,7 @@
         <v>57.017361111109494</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>45538.631944444445</v>
       </c>
@@ -3437,7 +3450,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>45539.614583333336</v>
       </c>
@@ -3455,7 +3468,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>45540.614583333336</v>
       </c>
@@ -3473,7 +3486,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>45541.614583333336</v>
       </c>
@@ -3491,7 +3504,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>45542.614583333336</v>
       </c>
@@ -3509,7 +3522,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>45543.614583333336</v>
       </c>
@@ -3527,7 +3540,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>45544.614583333336</v>
       </c>
@@ -3545,7 +3558,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>45545.614583333336</v>
       </c>
@@ -3563,7 +3576,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>45546.614583333336</v>
       </c>
@@ -3581,7 +3594,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>45547.614583333336</v>
       </c>
@@ -3599,7 +3612,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>45548.614583333336</v>
       </c>
@@ -3617,7 +3630,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>45549.614583333336</v>
       </c>
@@ -3635,7 +3648,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>45550.614583333336</v>
       </c>
@@ -3653,7 +3666,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>45551.614583333336</v>
       </c>
@@ -3671,7 +3684,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>45552.614583333336</v>
       </c>
@@ -3689,7 +3702,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>45553.614583333336</v>
       </c>
@@ -3707,7 +3720,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>45554.614583333336</v>
       </c>
@@ -3725,7 +3738,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>45555.614583333336</v>
       </c>
@@ -3743,7 +3756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>45556.614583333336</v>
       </c>
@@ -3761,7 +3774,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>45557.614583333336</v>
       </c>
@@ -3779,7 +3792,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>45558.614583333336</v>
       </c>
@@ -3797,7 +3810,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>45559.614583333336</v>
       </c>
@@ -3815,7 +3828,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>45560.614583333336</v>
       </c>
@@ -3833,7 +3846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>45561.614583333336</v>
       </c>
@@ -3851,7 +3864,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>45562.614583333336</v>
       </c>
@@ -3869,7 +3882,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>45563.614583333336</v>
       </c>
@@ -3887,7 +3900,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>45564.614583333336</v>
       </c>
@@ -3905,7 +3918,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>45565.614583333336</v>
       </c>
@@ -3923,161 +3936,161 @@
         <v>-45481.614583333336</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="C87" s="8"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
     </row>
   </sheetData>
@@ -4091,55 +4104,59 @@
   <dimension ref="A2:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="16" width="10.77734375" customWidth="1"/>
+    <col min="2" max="16" width="10.75" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="15.75">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="H2" s="40" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="H2" s="39" t="s">
         <v>26</v>
       </c>
       <c r="J2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1"/>
-    <row r="5" spans="1:17" ht="21" thickBot="1">
-      <c r="B5" s="41" t="s">
+    <row r="4" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="46"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>5</v>
       </c>
@@ -4192,7 +4209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>45481.614583333336</v>
       </c>
@@ -4211,7 +4228,7 @@
       <c r="F7" s="21">
         <v>1E-3</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <v>699.5</v>
       </c>
       <c r="H7" s="16">
@@ -4238,15 +4255,15 @@
       <c r="O7" s="16">
         <v>700.4</v>
       </c>
-      <c r="P7" s="32">
+      <c r="P7" s="31">
         <v>700.5</v>
       </c>
-      <c r="Q7" s="33">
+      <c r="Q7" s="32">
         <f>AVERAGE(G7:P7) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>700.58879999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>45482.621527777781</v>
       </c>
@@ -4265,7 +4282,7 @@
       <c r="F8" s="21">
         <v>1E-3</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="30">
         <v>641.1</v>
       </c>
       <c r="H8" s="16">
@@ -4292,15 +4309,15 @@
       <c r="O8" s="16">
         <v>640.9</v>
       </c>
-      <c r="P8" s="32">
+      <c r="P8" s="31">
         <v>640.9</v>
       </c>
-      <c r="Q8" s="33">
+      <c r="Q8" s="32">
         <f>AVERAGE(G8:P8) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>640.97899999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>45483.607638888891</v>
       </c>
@@ -4319,7 +4336,7 @@
       <c r="F9" s="21">
         <v>0.17599999999999999</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="30">
         <v>586.4</v>
       </c>
       <c r="H9" s="16">
@@ -4346,15 +4363,15 @@
       <c r="O9" s="16">
         <v>586.5</v>
       </c>
-      <c r="P9" s="32">
+      <c r="P9" s="31">
         <v>586.70000000000005</v>
       </c>
-      <c r="Q9" s="33">
+      <c r="Q9" s="32">
         <f>AVERAGE(G9:P9) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>586.29380000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>45484.613194444442</v>
       </c>
@@ -4373,7 +4390,7 @@
       <c r="F10" s="21">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="30">
         <v>537.79999999999995</v>
       </c>
       <c r="H10" s="16">
@@ -4400,15 +4417,15 @@
       <c r="O10" s="16">
         <v>537.6</v>
       </c>
-      <c r="P10" s="32">
+      <c r="P10" s="31">
         <v>537.4</v>
       </c>
-      <c r="Q10" s="33">
+      <c r="Q10" s="32">
         <f>AVERAGE(G10:P10) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>537.69180000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>45485.576388888891</v>
       </c>
@@ -4427,7 +4444,7 @@
       <c r="F11" s="21">
         <v>2E-3</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="30">
         <v>496.4</v>
       </c>
       <c r="H11" s="16">
@@ -4454,15 +4471,15 @@
       <c r="O11" s="16">
         <v>496.5</v>
       </c>
-      <c r="P11" s="32">
+      <c r="P11" s="31">
         <v>496.5</v>
       </c>
-      <c r="Q11" s="33">
+      <c r="Q11" s="32">
         <f>AVERAGE(G11:P11) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>495.95819999999992</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>45487.914583333331</v>
       </c>
@@ -4481,7 +4498,7 @@
       <c r="F12" s="21">
         <v>0</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="30">
         <v>404.4</v>
       </c>
       <c r="H12" s="16">
@@ -4508,15 +4525,15 @@
       <c r="O12" s="16">
         <v>404.4</v>
       </c>
-      <c r="P12" s="32">
+      <c r="P12" s="31">
         <v>404.4</v>
       </c>
-      <c r="Q12" s="33">
+      <c r="Q12" s="32">
         <f>AVERAGE(G12:P12) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>404.3698</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>45488.652777777781</v>
       </c>
@@ -4535,7 +4552,7 @@
       <c r="F13" s="21">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="30">
         <v>379.3</v>
       </c>
       <c r="H13" s="16">
@@ -4562,15 +4579,15 @@
       <c r="O13" s="16">
         <v>379.4</v>
       </c>
-      <c r="P13" s="32">
+      <c r="P13" s="31">
         <v>379.4</v>
       </c>
-      <c r="Q13" s="33">
+      <c r="Q13" s="32">
         <f>AVERAGE(G13:P13) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>379.36540000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>45490.597222222219</v>
       </c>
@@ -4589,7 +4606,7 @@
       <c r="F14" s="21">
         <v>0</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="30">
         <v>324.2</v>
       </c>
       <c r="H14" s="16">
@@ -4616,15 +4633,15 @@
       <c r="O14" s="16">
         <v>324.39999999999998</v>
       </c>
-      <c r="P14" s="32">
+      <c r="P14" s="31">
         <v>324.39999999999998</v>
       </c>
-      <c r="Q14" s="33">
+      <c r="Q14" s="32">
         <f>AVERAGE(G14:P14) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>324.31940000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>45492.756944444445</v>
       </c>
@@ -4643,7 +4660,7 @@
       <c r="F15" s="21">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="30">
         <v>266.60000000000002</v>
       </c>
       <c r="H15" s="16">
@@ -4670,15 +4687,15 @@
       <c r="O15" s="16">
         <v>266.60000000000002</v>
       </c>
-      <c r="P15" s="32">
+      <c r="P15" s="31">
         <v>266.60000000000002</v>
       </c>
-      <c r="Q15" s="33">
+      <c r="Q15" s="32">
         <f>AVERAGE(G15:P15) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>266.59579999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>45494.637499999997</v>
       </c>
@@ -4697,7 +4714,7 @@
       <c r="F16" s="21">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="30">
         <v>226.5</v>
       </c>
       <c r="H16" s="16">
@@ -4724,15 +4741,15 @@
       <c r="O16" s="16">
         <v>226.6</v>
       </c>
-      <c r="P16" s="32">
+      <c r="P16" s="31">
         <v>226.6</v>
       </c>
-      <c r="Q16" s="33">
+      <c r="Q16" s="32">
         <f>AVERAGE(G16:P16) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>226.57639999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>45496.621527777781</v>
       </c>
@@ -4751,7 +4768,7 @@
       <c r="F17" s="21">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="30">
         <v>191</v>
       </c>
       <c r="H17" s="16">
@@ -4778,15 +4795,15 @@
       <c r="O17" s="16">
         <v>190.9</v>
       </c>
-      <c r="P17" s="32">
+      <c r="P17" s="31">
         <v>190.9</v>
       </c>
-      <c r="Q17" s="33">
+      <c r="Q17" s="32">
         <f>AVERAGE(G17:P17) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>190.94220000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>45498.78402777778</v>
       </c>
@@ -4805,7 +4822,7 @@
       <c r="F18" s="21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="30">
         <v>158.69999999999999</v>
       </c>
       <c r="H18" s="16">
@@ -4832,15 +4849,15 @@
       <c r="O18" s="16">
         <v>158.5</v>
       </c>
-      <c r="P18" s="32">
+      <c r="P18" s="31">
         <v>158.5</v>
       </c>
-      <c r="Q18" s="33">
+      <c r="Q18" s="32">
         <f>AVERAGE(G18:P18) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>158.53600000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>45499.251388888886</v>
       </c>
@@ -4859,7 +4876,7 @@
       <c r="F19" s="21">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="30">
         <v>152.4</v>
       </c>
       <c r="H19" s="16">
@@ -4886,15 +4903,15 @@
       <c r="O19" s="16">
         <v>152.6</v>
       </c>
-      <c r="P19" s="32">
+      <c r="P19" s="31">
         <v>152.6</v>
       </c>
-      <c r="Q19" s="33">
+      <c r="Q19" s="32">
         <f>AVERAGE(G19:P19) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>152.49599999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>45502.631944444445</v>
       </c>
@@ -4913,7 +4930,7 @@
       <c r="F20" s="21">
         <v>1.2E-2</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="30">
         <v>115.2</v>
       </c>
       <c r="H20" s="16">
@@ -4940,73 +4957,73 @@
       <c r="O20" s="16">
         <v>115</v>
       </c>
-      <c r="P20" s="32">
+      <c r="P20" s="31">
         <v>115</v>
       </c>
-      <c r="Q20" s="33">
+      <c r="Q20" s="32">
         <f>AVERAGE(G20:P20) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>115.0384</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>45504.940972222219</v>
       </c>
-      <c r="B21" s="37">
+      <c r="B21" s="36">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="34">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="34">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="34">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="37">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="33">
         <v>93.61</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="34">
         <v>93.62</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="34">
         <v>93.65</v>
       </c>
-      <c r="J21" s="35">
+      <c r="J21" s="34">
         <v>93.65</v>
       </c>
-      <c r="K21" s="35">
+      <c r="K21" s="34">
         <v>93.65</v>
       </c>
-      <c r="L21" s="35">
+      <c r="L21" s="34">
         <v>93.64</v>
       </c>
-      <c r="M21" s="35">
+      <c r="M21" s="34">
         <v>93.65</v>
       </c>
-      <c r="N21" s="35">
+      <c r="N21" s="34">
         <v>93.65</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="34">
         <v>93.63</v>
       </c>
-      <c r="P21" s="36">
+      <c r="P21" s="35">
         <v>93.64</v>
       </c>
-      <c r="Q21" s="33">
+      <c r="Q21" s="32">
         <f>AVERAGE(G21:P21) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>93.633199999999988</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>45509.602777777778</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="30">
         <v>2E-3</v>
       </c>
       <c r="C22" s="16">
@@ -5018,7 +5035,7 @@
       <c r="E22" s="16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="31">
         <v>2E-3</v>
       </c>
       <c r="G22" s="17">
@@ -5048,19 +5065,19 @@
       <c r="O22" s="16">
         <v>62.61</v>
       </c>
-      <c r="P22" s="32">
+      <c r="P22" s="31">
         <v>62.62</v>
       </c>
-      <c r="Q22" s="33">
+      <c r="Q22" s="32">
         <f>AVERAGE(G22:P22) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>62.613199999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>45512.597222222219</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="30">
         <v>1.4E-2</v>
       </c>
       <c r="C23" s="16">
@@ -5072,7 +5089,7 @@
       <c r="E23" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="31">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G23" s="17">
@@ -5102,7 +5119,7 @@
       <c r="O23" s="16">
         <v>49.24</v>
       </c>
-      <c r="P23" s="32">
+      <c r="P23" s="31">
         <v>49.25</v>
       </c>
       <c r="Q23" s="21">
@@ -5110,11 +5127,11 @@
         <v>49.233000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>45516.676388888889</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="30">
         <v>1.2E-2</v>
       </c>
       <c r="C24" s="16">
@@ -5126,7 +5143,7 @@
       <c r="E24" s="16">
         <v>0.01</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="31">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G24" s="17">
@@ -5156,7 +5173,7 @@
       <c r="O24" s="16">
         <v>34.18</v>
       </c>
-      <c r="P24" s="32">
+      <c r="P24" s="31">
         <v>34.19</v>
       </c>
       <c r="Q24" s="21">
@@ -5164,11 +5181,11 @@
         <v>34.167000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>45519.638888888891</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="30">
         <v>1.2E-2</v>
       </c>
       <c r="C25" s="16">
@@ -5180,7 +5197,7 @@
       <c r="E25" s="16">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="31">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="G25" s="17">
@@ -5210,7 +5227,7 @@
       <c r="O25" s="16">
         <v>26.58</v>
       </c>
-      <c r="P25" s="32">
+      <c r="P25" s="31">
         <v>26.57</v>
       </c>
       <c r="Q25" s="21">
@@ -5218,11 +5235,11 @@
         <v>26.585799999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>45523.675000000003</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="30">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="C26" s="16">
@@ -5234,7 +5251,7 @@
       <c r="E26" s="16">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="31">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G26" s="17">
@@ -5264,7 +5281,7 @@
       <c r="O26" s="16">
         <v>18.41</v>
       </c>
-      <c r="P26" s="32">
+      <c r="P26" s="31">
         <v>18.41</v>
       </c>
       <c r="Q26" s="21">
@@ -5272,11 +5289,11 @@
         <v>18.400599999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <v>45526.636111111111</v>
       </c>
-      <c r="B27" s="31">
+      <c r="B27" s="30">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="C27" s="16">
@@ -5288,7 +5305,7 @@
       <c r="E27" s="16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="31">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G27" s="17">
@@ -5318,7 +5335,7 @@
       <c r="O27" s="16">
         <v>14.27</v>
       </c>
-      <c r="P27" s="32">
+      <c r="P27" s="31">
         <v>14.27</v>
       </c>
       <c r="Q27" s="21">
@@ -5326,11 +5343,11 @@
         <v>14.269600000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>45530.602083333331</v>
       </c>
-      <c r="B28" s="31">
+      <c r="B28" s="30">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="C28" s="16">
@@ -5342,7 +5359,7 @@
       <c r="E28" s="16">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="31">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="G28" s="17">
@@ -5372,7 +5389,7 @@
       <c r="O28" s="16">
         <v>10.130000000000001</v>
       </c>
-      <c r="P28" s="32">
+      <c r="P28" s="31">
         <v>10.130000000000001</v>
       </c>
       <c r="Q28" s="21">
@@ -5380,100 +5397,132 @@
         <v>10.122199999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="26">
         <v>45538.633333333331</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="34">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D29" s="35">
+      <c r="D29" s="34">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="34">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F29" s="36">
+      <c r="F29" s="35">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G29" s="37">
+      <c r="G29" s="36">
         <v>5.0830000000000002</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="34">
         <v>5.0759999999999996</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I29" s="34">
         <v>5.077</v>
       </c>
-      <c r="J29" s="35">
+      <c r="J29" s="34">
         <v>5.07</v>
       </c>
-      <c r="K29" s="35">
+      <c r="K29" s="34">
         <v>5.0709999999999997</v>
       </c>
-      <c r="L29" s="35">
+      <c r="L29" s="34">
         <v>5.0720000000000001</v>
       </c>
-      <c r="M29" s="35">
+      <c r="M29" s="34">
         <v>5.0739999999999998</v>
       </c>
-      <c r="N29" s="35">
+      <c r="N29" s="34">
         <v>5.0730000000000004</v>
       </c>
-      <c r="O29" s="35">
+      <c r="O29" s="34">
         <v>5.07</v>
       </c>
-      <c r="P29" s="36">
+      <c r="P29" s="35">
         <v>5.0739999999999998</v>
       </c>
-      <c r="Q29" s="38">
+      <c r="Q29" s="37">
         <f>AVERAGE(G29:P29) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>5.0691999999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="25"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="21" t="e">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="25">
+        <v>45547.556944444441</v>
+      </c>
+      <c r="B30" s="30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="D30" s="16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0</v>
+      </c>
+      <c r="F30" s="31">
+        <v>0</v>
+      </c>
+      <c r="G30" s="17">
+        <v>2.343</v>
+      </c>
+      <c r="H30" s="16">
+        <v>2.355</v>
+      </c>
+      <c r="I30" s="16">
+        <v>2.3660000000000001</v>
+      </c>
+      <c r="J30" s="16">
+        <v>2.3719999999999999</v>
+      </c>
+      <c r="K30" s="16">
+        <v>2.371</v>
+      </c>
+      <c r="L30" s="16">
+        <v>2.367</v>
+      </c>
+      <c r="M30" s="16">
+        <v>2.3690000000000002</v>
+      </c>
+      <c r="N30" s="16">
+        <v>2.3679999999999999</v>
+      </c>
+      <c r="O30" s="16">
+        <v>2.367</v>
+      </c>
+      <c r="P30" s="31">
+        <v>2.3660000000000001</v>
+      </c>
+      <c r="Q30" s="21">
         <f>AVERAGE(G30:P30) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+        <v>2.3633999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="38" t="e">
+      <c r="B31" s="33"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="37" t="e">
         <f>AVERAGE(G31:P31) - AVERAGE(Tabulka1[[#This Row],[č.1]:[č.5]])</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>